<commit_message>
temoa_stochastic - added EmissionLimitMultiplier
Revised va_stoch scenarios to focus on EmissionLimitMultiplier
</commit_message>
<xml_diff>
--- a/projects/va_stoch/data/data_va_stochEmerg.xlsx
+++ b/projects/va_stoch/data/data_va_stochEmerg.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358846D1-8F2F-4175-BF53-9C1DA92E82AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92A3E77-C81C-4E22-AC5E-2E4F60E08ACF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="844" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -3805,7 +3805,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C13" sqref="C13:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4280,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="2" t="str">
-        <f>D15</f>
+        <f t="shared" ref="G15:G25" si="1">D15</f>
         <v>NREL ATB, 2020, Dedicated</v>
       </c>
       <c r="H15" s="48">
@@ -4316,7 +4316,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="str">
-        <f>D16</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, new</v>
       </c>
       <c r="H16" s="48">
@@ -4326,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f t="shared" ref="J16:J27" si="1">G16</f>
+        <f t="shared" ref="J16:J27" si="2">G16</f>
         <v>NREL ATB, 2020, new</v>
       </c>
       <c r="K16" s="2"/>
@@ -4352,7 +4352,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="str">
-        <f>D17</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, NG_CC</v>
       </c>
       <c r="H17" s="48">
@@ -4362,7 +4362,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, NG_CC</v>
       </c>
       <c r="K17" s="2"/>
@@ -4388,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="2" t="str">
-        <f>D18</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, NG_CC</v>
       </c>
       <c r="H18" s="48">
@@ -4398,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, NG_CC</v>
       </c>
       <c r="K18" s="2"/>
@@ -4424,7 +4424,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="2" t="str">
-        <f>D19</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, NG_CT</v>
       </c>
       <c r="H19" s="48">
@@ -4434,7 +4434,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, NG_CT</v>
       </c>
       <c r="K19" s="2"/>
@@ -4460,7 +4460,7 @@
         <v>-2.2566511329908701</v>
       </c>
       <c r="G20" s="2" t="str">
-        <f>D20</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, Utility</v>
       </c>
       <c r="H20" s="48">
@@ -4470,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, Utility</v>
       </c>
       <c r="K20" s="2">
@@ -4500,7 +4500,7 @@
         <v>-2.4441204658121647</v>
       </c>
       <c r="G21" s="2" t="str">
-        <f>D21</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, Cl4</v>
       </c>
       <c r="H21" s="48">
@@ -4510,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, Cl4</v>
       </c>
       <c r="K21" s="2">
@@ -4540,7 +4540,7 @@
         <v>-2.611397438874592</v>
       </c>
       <c r="G22" s="2" t="str">
-        <f>D22</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, Commercial</v>
       </c>
       <c r="H22" s="48">
@@ -4550,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, Commercial</v>
       </c>
       <c r="K22" s="2">
@@ -4580,7 +4580,7 @@
         <v>-2.4437991514549156</v>
       </c>
       <c r="G23" s="2" t="str">
-        <f>D23</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, Cl12</v>
       </c>
       <c r="H23" s="48">
@@ -4590,7 +4590,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, Cl12</v>
       </c>
       <c r="K23" s="2">
@@ -4620,7 +4620,7 @@
         <v>-3.7531641335752619</v>
       </c>
       <c r="G24" s="2" t="str">
-        <f>D24</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, 2020, Residential</v>
       </c>
       <c r="H24" s="48">
@@ -4630,7 +4630,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, 2020, Residential</v>
       </c>
       <c r="K24" s="2">
@@ -4660,7 +4660,7 @@
         <v>-1.0317377259688025</v>
       </c>
       <c r="G25" s="2" t="str">
-        <f>D25</f>
+        <f t="shared" si="1"/>
         <v>NREL ATB, Gas-CC-CC, 2025</v>
       </c>
       <c r="H25" s="51">
@@ -4670,7 +4670,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>NREL ATB, Gas-CC-CC, 2025</v>
       </c>
       <c r="K25" s="2"/>
@@ -4705,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>APEN paper, incr assumed constant</v>
       </c>
       <c r="K26" s="2"/>
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Projection</v>
       </c>
       <c r="K27" s="2"/>

</xml_diff>